<commit_message>
Updated data in old records.
</commit_message>
<xml_diff>
--- a/script_for_suprim_court_data/dataset.xlsx
+++ b/script_for_suprim_court_data/dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,78 +484,84 @@
           <t>पूर्ण पाठ</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>आदेश /फैसलाको किसिम</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>६</t>
+          <t>११</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>०६९-RC-००८३</t>
+          <t>०६९-WO-११४५</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>११८५७१</t>
+          <t>११८८४०</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-१६</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>फौजदारी</t>
+          <t>रिट निवेदन</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>कर्तव्य ज्यान</t>
+          <t>उत्प्रेषण</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>नेपाल सरकार</t>
+          <t>निरञ्जना योगी</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>धनबहादुर शाही</t>
+          <t>स्वास्थ्य तथा जनसंख्या मन्त्रालय समेत ३</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>२०७०-०३-०५</t>
+          <t>२०७१-०८-२८</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118571.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118840.pdf</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>१२</t>
+          <t>१४</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>०६९-WO-११०१</t>
+          <t>०६९-WO-११४४</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>११८५३४</t>
+          <t>११८८३४</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-१६</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -570,44 +576,45 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>रामरतन थारु</t>
+          <t>नर्वदेश्वर शुक्ल</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>पुनरावेदन अदालत नेपालगंज समेत ५</t>
+          <t>जिल्ला शिक्षा कार्यालय पाल्पा समेत ३</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>२०७१-१०-०८</t>
+          <t>२०७२-०३-०१</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118534.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118834.pdf</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>१७</t>
+          <t>१५</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>०६९-WO-१०९९</t>
+          <t>०६९-WO-११४७</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>११८५३२</t>
+          <t>११८८४९</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-१६</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -622,24 +629,25 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>भिखारी राउत कुर्मी</t>
+          <t>शुसिला दाहाल मास्के</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>पुनरावेदन अदालत हेटौडा समेत ४</t>
+          <t>पुनरावेदन अदालत पाटन समेत ५</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>२०७३-०४-२७</t>
+          <t>२०७२-१०-०७</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118532.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118849.pdf</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -649,17 +657,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>०६९-WO-११०२</t>
+          <t>०६९-WO-११४६</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>११८५३६</t>
+          <t>११८८४६</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-१६</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -674,44 +682,45 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>प्रदिप घिमिरे</t>
+          <t>राधेश्याम कार्की</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>काठमाण्डौ विश्व वद्यालिय धुलिखेल समेत ६</t>
+          <t>मालपोत कार्यालय चाबहील समेत ४</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>२०७३-०३-१४</t>
+          <t>२०७५-०३-२०</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118536.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118846.pdf</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>२६</t>
+          <t>१९</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>०६९-WO-११००</t>
+          <t>०६९-WO-११४८</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>११८५३३</t>
+          <t>११८८५४</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-१६</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -726,44 +735,45 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>रमेश प्रधान समेत ४५</t>
+          <t>शम्भु प्रसाद साह</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>सम्माननीय अध्यक्ष प्रधानमन्त्रि तथा मन्त्रपिरिषदको कार्यालय समेत १२</t>
+          <t>जिल्ला शिक्षा कार्यालय ओखलढुङ्गा समेत ६</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>२०७४-१०-१५</t>
+          <t>२०७५-०७-१३</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118533.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118854.pdf</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>२७</t>
+          <t>२०</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>०६९-CR-०८००</t>
+          <t>०६९-CR-०८३३</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>११८५३९</t>
+          <t>११८९२४</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-१६</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -773,12 +783,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>भ्रष्टाचार</t>
+          <t>कर्तव्य ज्यान</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>भुना पोखरेल</t>
+          <t>सन्त बहादुर थापा मगर</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -788,86 +798,88 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>२०७५-०५-२८</t>
+          <t>२०७६-०३-०२</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118539.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118924.pdf</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>२८</t>
+          <t>२१</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>०६९-WO-१०९६</t>
+          <t>०६९-CR-०८३४</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>११८५२३</t>
+          <t>११८९२६</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-१६</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>रिट निवेदन</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>उत्प्रेषण</t>
+          <t>कर्तव्य ज्यान</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>महेन्द्र प्रसाद यादव</t>
+          <t>टंक बहादुर थापा मगर</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>कृषि बिकास बैंक लि।मुख्य कार्यालय रामशाहपथ काठमाडौं समेत ४</t>
+          <t>नेपाल सरकार</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>२०७५-०७-१८</t>
+          <t>२०७६-०३-०२</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118523.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118926.pdf</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>२९</t>
+          <t>१२</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>०६९-WO-१०९८</t>
+          <t>०६९-WO-१०९४</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>११८५३१</t>
+          <t>११८४९८</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -882,44 +894,45 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>गुणादेवी लामीछाने</t>
+          <t>दिपक कुमार गुप्ता</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>शिक्षा मन्त्रालय सिंहदरवार समेत ७</t>
+          <t>भौतीक पूर्वाधार तथा यातायात ब्यबस्था मन्त्रालय समेत ७</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>२०७७-०८-२५</t>
+          <t>२०७०-०८-२५</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118531.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118498.pdf</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>३०</t>
+          <t>१८</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>०६९-CI-०९९२</t>
+          <t>०६९-CI-०९८३</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>११८५५३</t>
+          <t>११८५४०</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -929,96 +942,98 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>नामसारी</t>
+          <t>निषेधाज्ञा</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>रामदेव साह तेली</t>
+          <t>अम्रिका पासी र सत्यनारायण पासी</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>तपसी साह तेली</t>
+          <t>जिलेदार पासी</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>२०७९-०६-२४</t>
+          <t>२०७२-०३-०८</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118553.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118540.pdf</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>३१</t>
+          <t>१९</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>०६९-CI-०९९३</t>
+          <t>०६९-CR-०७९७</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>११८५५७</t>
+          <t>११८५२६</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>२०७०-०१-०३</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>देवानी</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>लिखत वदर</t>
+          <t>सम्बन्धविच्छेद</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>मानो देवी साह</t>
+          <t>सावित्रि देवी पाठक , भगौती प्रसाद पाठक , आफ्नो हकमा समेत कप्तान कुमार पाठक र राजेश कुमार पाठक</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>तपसी साह तेली</t>
+          <t>उमा देवी पाठक</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>२०७९-०६-२४</t>
+          <t>२०७२-०३-३१</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118557.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118526.pdf</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>१२</t>
+          <t>२०</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>०६९-WO-१०९४</t>
+          <t>०६९-CI-०९८६</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>११८४९८</t>
+          <t>११८५४३</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1028,7 +1043,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>रिट निवेदन</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1038,39 +1053,40 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>दिपक कुमार गुप्ता</t>
+          <t>भुपेन्द्र शाही</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>भौतीक पूर्वाधार तथा यातायात ब्यबस्था मन्त्रालय समेत ७</t>
+          <t>श्री मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज , श्री अध्यक्ष मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज र श्री कार्यकारी प्रमुख मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>२०७०-०८-२५</t>
+          <t>२०७२-०४-१७</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118498.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118543.pdf</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>१८</t>
+          <t>२६</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>०६९-CI-०९८३</t>
+          <t>०६९-CR-०७९८</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>११८५४०</t>
+          <t>११८५३७</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1080,49 +1096,50 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>देवानी</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>निषेधाज्ञा</t>
+          <t>लागु ‌‌औषधी हिरोइन</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>अम्रिका पासी र सत्यनारायण पासी</t>
+          <t>बलबहादुर सारु मगर</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>जिलेदार पासी</t>
+          <t>नेपाल सरकार</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>२०७२-०३-०८</t>
+          <t>२०७२-०८-२०</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118540.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118537.pdf</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>१९</t>
+          <t>२९</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>०६९-CR-०७९७</t>
+          <t>०६९-CI-०९९१</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>११८५२६</t>
+          <t>११८५५०</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1132,49 +1149,50 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>फौजदारी</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>सम्बन्धविच्छेद</t>
+          <t>परमादेश</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>सावित्रि देवी पाठक , भगौती प्रसाद पाठक , आफ्नो हकमा समेत कप्तान कुमार पाठक र राजेश कुमार पाठक</t>
+          <t>राम सागर मुराउ</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>उमा देवी पाठक</t>
+          <t>हिरमिनिया गाउं विकास समितिको कार्यालय बांके र ऐ।गा।वि।स। का सचिव एवं अध्यक्ष ऋषिराज गौतम</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>२०७२-०३-३१</t>
+          <t>२०७३-०५-१९</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118526.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118550.pdf</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>२०</t>
+          <t>३१</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>०६९-CI-०९८६</t>
+          <t>०६९-CI-०९९०</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>११८५४३</t>
+          <t>११८५४९</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1189,44 +1207,45 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>उत्प्रेषण</t>
+          <t>जग्गा खिचोला</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>भुपेन्द्र शाही</t>
+          <t>सोनेलाल मण्डल भन्ने सोनमा मण्डल</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>श्री मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज , श्री अध्यक्ष मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज र श्री कार्यकारी प्रमुख मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज</t>
+          <t>लक्ष्मण मण्डल</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>२०७२-०४-१७</t>
+          <t>२०७३-११-२२</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118543.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118549.pdf</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>२६</t>
+          <t>३३</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>०६९-CR-०७९८</t>
+          <t>०६९-CI-०९८५</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>११८५३७</t>
+          <t>११८५४२</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1236,49 +1255,50 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>फौजदारी</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>लागु ‌‌औषधी हिरोइन</t>
+          <t>अन्य</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>बलबहादुर सारु मगर</t>
+          <t>केशवराम यादव अहिर</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>नेपाल सरकार</t>
+          <t>स्वामी दयाल अहिर , रामेश्वर अहिर , सुधरी अहिर , हौसिलाल अहिर , प्यारा अहिर , पुलईराम अहिर र गया प्रसाद अहिर</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>२०७२-०८-२०</t>
+          <t>२०७४-१०-१५</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118537.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118542.pdf</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>२९</t>
+          <t>३४</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>०६९-CI-०९९१</t>
+          <t>०६९-CI-०९८८</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>११८५५०</t>
+          <t>११८५४५</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1293,44 +1313,45 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>परमादेश</t>
+          <t>अन्य</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>राम सागर मुराउ</t>
+          <t>सुघरी अहिर , प्यारा अहिर र आफ्नो हकमा समेत जबाहरलाल अहिर</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>हिरमिनिया गाउं विकास समितिको कार्यालय बांके र ऐ।गा।वि।स। का सचिव एवं अध्यक्ष ऋषिराज गौतम</t>
+          <t>केशव राम अहिर</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>२०७३-०५-१९</t>
+          <t>२०७४-१०-१५</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118550.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118545.pdf</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>३१</t>
+          <t>३५</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>०६९-CI-०९९०</t>
+          <t>०६९-CI-०९८४</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>११८५४९</t>
+          <t>११८५४१</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1345,44 +1366,45 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>जग्गा खिचोला</t>
+          <t>अन्य</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>सोनेलाल मण्डल भन्ने सोनमा मण्डल</t>
+          <t>मुख्तार अली वागवान</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>लक्ष्मण मण्डल</t>
+          <t>मुमताज वागवान</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>२०७३-११-२२</t>
+          <t>२०७४-१०-०५</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118549.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118541.pdf</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>३३</t>
+          <t>३६</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>०६९-CI-०९८५</t>
+          <t>०६९-CI-०९८९</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>११८५४२</t>
+          <t>११८५४८</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1397,44 +1419,45 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>अन्य</t>
+          <t>जग्गा खिचोला</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>केशवराम यादव अहिर</t>
+          <t>चेतराम भुजुवा</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>स्वामी दयाल अहिर , रामेश्वर अहिर , सुधरी अहिर , हौसिलाल अहिर , प्यारा अहिर , पुलईराम अहिर र गया प्रसाद अहिर</t>
+          <t>पटवारी पथरकट</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>२०७४-१०-१५</t>
+          <t>२०७५-०३-०८</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118542.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118548.pdf</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>३४</t>
+          <t>३७</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>०६९-CI-०९८८</t>
+          <t>०६९-CR-०७९९</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>११८५४५</t>
+          <t>११८५३८</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1444,49 +1467,50 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>देवानी</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>अन्य</t>
+          <t>अपहरण तथा शरिर बन्धक</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>सुघरी अहिर , प्यारा अहिर र आफ्नो हकमा समेत जबाहरलाल अहिर</t>
+          <t>दिल कुमारी लावती</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>केशव राम अहिर</t>
+          <t>नेपाल सरकार</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>२०७४-१०-१५</t>
+          <t>२०७६-०८-१६</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118545.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118538.pdf</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>३५</t>
+          <t>३८</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>०६९-CI-०९८४</t>
+          <t>०६९-CI-०९८७</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>११८५४१</t>
+          <t>११८५४४</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1501,44 +1525,45 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>अन्य</t>
+          <t>जग्गा खिचोला</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>मुख्तार अली वागवान</t>
+          <t>रामगोपाल थारु</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>मुमताज वागवान</t>
+          <t>निरु देवी मेचे</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>२०७४-१०-०५</t>
+          <t>२०७७-०४-१३</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118541.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118544.pdf</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>३६</t>
+          <t>१२</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>०६९-CI-०९८९</t>
+          <t>०६९-WO-१०९४</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>११८५४८</t>
+          <t>११८४९८</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1548,49 +1573,50 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>देवानी</t>
+          <t>रिट निवेदन</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>जग्गा खिचोला</t>
+          <t>उत्प्रेषण</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>चेतराम भुजुवा</t>
+          <t>दिपक कुमार गुप्ता</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>पटवारी पथरकट</t>
+          <t>भौतीक पूर्वाधार तथा यातायात ब्यबस्था मन्त्रालय समेत ७</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>२०७५-०३-०८</t>
+          <t>२०७०-०८-२५</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118548.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118498.pdf</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>३७</t>
+          <t>१८</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>०६९-CR-०७९९</t>
+          <t>०६९-CI-०९८३</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>११८५३८</t>
+          <t>११८५४०</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1600,49 +1626,50 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>फौजदारी</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>अपहरण तथा शरिर बन्धक</t>
+          <t>निषेधाज्ञा</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>दिल कुमारी लावती</t>
+          <t>अम्रिका पासी र सत्यनारायण पासी</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>नेपाल सरकार</t>
+          <t>जिलेदार पासी</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>२०७६-०८-१६</t>
+          <t>२०७२-०३-०८</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118538.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118540.pdf</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>३८</t>
+          <t>१९</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>०६९-CI-०९८७</t>
+          <t>०६९-CR-०७९७</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>११८५४४</t>
+          <t>११८५२६</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1652,106 +1679,108 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>देवानी</t>
+          <t>फौजदारी</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>जग्गा खिचोला</t>
+          <t>सम्बन्धविच्छेद</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>रामगोपाल थारु</t>
+          <t>सावित्रि देवी पाठक , भगौती प्रसाद पाठक , आफ्नो हकमा समेत कप्तान कुमार पाठक र राजेश कुमार पाठक</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>निरु देवी मेचे</t>
+          <t>उमा देवी पाठक</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>२०७७-०४-१३</t>
+          <t>२०७२-०३-३१</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118544.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118526.pdf</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>३</t>
+          <t>२०</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>०६९-CR-०८०६</t>
+          <t>०६९-CI-०९८६</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>११८६६७</t>
+          <t>११८५४३</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>२०७०-०१-०५</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>फौजदारी</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>वन्दीप्रत्यक्षीकरण</t>
+          <t>उत्प्रेषण</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>दलबहादुर याखा</t>
+          <t>भुपेन्द्र शाही</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>जल्लिा धनकुटा, धनकुटा न।पा। वडा नं। ४ स्िथत धनकुटा जल्लिा अदालत धनकुटा , ऐ। धनकुटा जिल्ला अदालत तहशिल शाखा , ऐ। धनकुटा जिल्ला प्रहरी कार्यालय धनकुटा र कारागार कार्यालय धनकुटा</t>
+          <t>श्री मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज , श्री अध्यक्ष मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज र श्री कार्यकारी प्रमुख मध्य पश्चमिाञ्चल ग्रामिण विकास बैंक प्रधान कार्यालय नेपालगंज</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>२०७०-१२-२३</t>
+          <t>२०७२-०४-१७</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118667.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118543.pdf</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>७</t>
+          <t>२६</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>०६९-CR-०८१२</t>
+          <t>०६९-CR-०७९८</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>११८८०४</t>
+          <t>११८५३७</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>२०७०-०१-०५</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1761,12 +1790,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>कर्तव्य ज्यान</t>
+          <t>लागु ‌‌औषधी हिरोइन</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>रामचन्द्र श्रेष्ठ</t>
+          <t>बलबहादुर सारु मगर</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1776,138 +1805,141 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>२०७२-०६-०७</t>
+          <t>२०७२-०८-२०</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118804.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118537.pdf</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>११</t>
+          <t>२९</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>०६९-CR-०८१९</t>
+          <t>०६९-CI-०९९१</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>११८८४१</t>
+          <t>११८५५०</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>२०७०-०१-०९</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>फौजदारी</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>वैदेशिक रोजगार</t>
+          <t>परमादेश</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>युवराज दहाल</t>
+          <t>राम सागर मुराउ</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>नेपाल सरकार</t>
+          <t>हिरमिनिया गाउं विकास समितिको कार्यालय बांके र ऐ।गा।वि।स। का सचिव एवं अध्यक्ष ऋषिराज गौतम</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>२०७२-१२-१८</t>
+          <t>२०७३-०५-१९</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118841.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118550.pdf</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>२</t>
+          <t>३१</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>०६९-WO-११३१</t>
+          <t>०६९-CI-०९९०</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>११८७४०</t>
+          <t>११८५४९</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>२०७०-०१-१२</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>रिट निवेदन</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>उत्प्रेषण</t>
+          <t>जग्गा खिचोला</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>गोर्खा ब्रुअरी प्रा।ली।का अ।प्रा।सुरेन्द्र सिलवाल</t>
+          <t>सोनेलाल मण्डल भन्ने सोनमा मण्डल</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>श्रम अदालत अनामनगर समेत ३०</t>
+          <t>लक्ष्मण मण्डल</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>२०७०-११-२०</t>
+          <t>२०७३-११-२२</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118740.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118549.pdf</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>३</t>
+          <t>३३</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>०६९-CI-१०१५</t>
+          <t>०६९-CI-०९८५</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>११८८८१</t>
+          <t>११८५४२</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>२०७०-०१-१२</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1917,185 +1949,1885 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>परमादेश</t>
+          <t>अन्य</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>श्री बसवटि्ी गा।व।िस। को कार्यालय, बसवटि्ी, सप्तरी र ऐ। कार्यालयका सचिव रुन्दी यादव</t>
+          <t>केशवराम यादव अहिर</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>सकुर मियां , गुलशेर मियां र दिल महम्मद मियां</t>
+          <t>स्वामी दयाल अहिर , रामेश्वर अहिर , सुधरी अहिर , हौसिलाल अहिर , प्यारा अहिर , पुलईराम अहिर र गया प्रसाद अहिर</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>२०७०-११-१९</t>
+          <t>२०७४-१०-१५</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118881.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118542.pdf</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>१७</t>
+          <t>३४</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>०६९-CR-०८३२</t>
+          <t>०६९-CI-०९८८</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>११८९२२</t>
+          <t>११८५४५</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>२०७०-०१-१५</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>फौजदारी</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>सरकारीछाप र दस्तखत कीर्ते</t>
+          <t>अन्य</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>जगदिश देशार</t>
+          <t>सुघरी अहिर , प्यारा अहिर र आफ्नो हकमा समेत जबाहरलाल अहिर</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>नेपाल सरकार</t>
+          <t>केशव राम अहिर</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>२०७४-०२-२९</t>
+          <t>२०७४-१०-१५</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118922.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118545.pdf</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>१८</t>
+          <t>३५</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>०६९-WO-११४२</t>
+          <t>०६९-CI-०९८४</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>११८८००</t>
+          <t>११८५४१</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>२०७०-०१-१५</t>
+          <t>२०७०-०१-०२</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>रिट निवेदन</t>
+          <t>देवानी</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>उत्प्रेषण</t>
+          <t>अन्य</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>रामचन्द्र प्रसाद गुप्ता</t>
+          <t>मुख्तार अली वागवान</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>नेपाल विद्युत प्राधिकरण केन्द्रिय कार्यालय दरवारमार्ग समेत ७</t>
+          <t>मुमताज वागवान</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>२०७४-११-०८</t>
+          <t>२०७४-१०-०५</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118800.pdf</t>
-        </is>
-      </c>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118541.pdf</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>३६</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>०६९-CI-०९८९</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>११८५४८</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>२०७०-०१-०२</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>जग्गा खिचोला</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>चेतराम भुजुवा</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>पटवारी पथरकट</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>२०७५-०३-०८</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118548.pdf</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>३७</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>०६९-CR-०७९९</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>११८५३८</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>२०७०-०१-०२</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>अपहरण तथा शरिर बन्धक</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>दिल कुमारी लावती</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>२०७६-०८-१६</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118538.pdf</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>३८</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>०६९-CI-०९८७</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>११८५४४</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>२०७०-०१-०२</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>जग्गा खिचोला</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>रामगोपाल थारु</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>निरु देवी मेचे</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>२०७७-०४-१३</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118544.pdf</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>१३</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८८</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>१४१७२५</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>वहुविवाह</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>सन्तोष भन्ने लिला बहादुर गिरी र सम्झना भन्ने रेश्मा गिरी</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>२०७३-०५-२०</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141725.pdf</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>१४</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१८</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>१४१५०५</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>योग बहादुर पाल</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>प्रहरी प्रधान कार्यालय नक्साल समेत ३ र प्रहरी नायव महानिरिक्षक माधव प्रसाद जोशी</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>२०७३-०७-२४</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141505.pdf</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>१५</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८१</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>१४१७३२</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>निषेधाज्ञा</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>मिनादेवी गुप्ता</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>जयकुमार साह</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>२०७३-०६-०६</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141732.pdf</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>१६</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८९</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>१४१७२६</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>कर्तव्य ज्यान</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>लक्ष्मण धमला</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>२०७३-११-०८</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141726.pdf</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>१७</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८४</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>१४१७३६</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>परमादेश</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>जिल्ला प्रहरी कार्यालय मोरंग</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>गुदानी कुमार</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>२०७३-१२-१५</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141736.pdf</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>१८</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८५</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>१४१७३८</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>परमादेश</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>जिल्ला विकास समितिको कार्यालय कास्की</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>गुदानी कुमार</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>२०७३-१२-१५</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141738.pdf</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>१९</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>०६९-CI-१०३०</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>११८९०८</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>२०७०-०१-१५</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८५</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>१४१७१९</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>जवरजस्ती करणी</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>डिल्ली स्वार , राकेश कुँवर र ध्रुब कुँवर</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>२०७४-०१-२८</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141719.pdf</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>२०</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१६</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>१४१४८८</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>रतन कुमार श्रेष्ठ</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>मालपोत कार्यालय पर्सा , मालपोत कार्यालय पर्सा , अख्तियार दुरुपयोग अनुसन्धान आयोग टंगाल समेत ६ , लुम्बिनी विकास बैंक लिमिटेड भरतपुर , लुम्बिनी विकास बैंक लिमिटेड मकवानपुर , सुनिता महतो र सुभाषविर माथेमा</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>२०७४-०२-२६</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141488.pdf</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>२१</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१७</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>१४१४९०</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>दिपक कुमार श्रेष्ठ</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>मालपोत कार्यालय पर्सा , अख्तियार दुरुपयोग अनुसन्धान आयोग टंगाल समेत ६ , लुम्बिनी विकास बैंक लिमिटेड भरतपुर , लुम्बिनी विकास बैंक लिमिटेड मकवानपुर , सुनिता महतो र सुभाषविर माथेमा</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>२०७४-०२-२६</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141490.pdf</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>२४</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२७८</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>१४१७२७</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
         <is>
           <t>देवानी</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>अशं चलन</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>सुनमाया गुरुङ्गको अ।वा। दिल बहादुर सुनार</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>वीर बहादुर गुरुङ्ग</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>२०७४-०५-०६</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141727.pdf</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>१३</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८८</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>१४१७२५</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>वहुविवाह</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>सन्तोष भन्ने लिला बहादुर गिरी र सम्झना भन्ने रेश्मा गिरी</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>२०७३-०५-२०</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141725.pdf</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>१४</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१८</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>१४१५०५</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>योग बहादुर पाल</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>प्रहरी प्रधान कार्यालय नक्साल समेत ३ र प्रहरी नायव महानिरिक्षक माधव प्रसाद जोशी</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>२०७३-०७-२४</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141505.pdf</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>१५</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८१</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>१४१७३२</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>निषेधाज्ञा</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>मिनादेवी गुप्ता</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>जयकुमार साह</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>२०७३-०६-०६</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141732.pdf</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>१६</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८९</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>१४१७२६</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>कर्तव्य ज्यान</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>लक्ष्मण धमला</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>२०७३-११-०८</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141726.pdf</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>१७</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८४</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>१४१७३६</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
         <is>
           <t>परमादेश</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>चस्मती जग्गा एकीकरण आयोजनाको तर्फबाट अधिकार प्राप्त आयोजना प्रमुख रविन्द्र कुमार पौड्याल</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>उत्तम दास मानन्धर समेत ५ जना</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>२०७५-११-२९</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_118908.pdf</t>
-        </is>
-      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>जिल्ला प्रहरी कार्यालय मोरंग</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>गुदानी कुमार</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>२०७३-१२-१५</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141736.pdf</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>१८</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८५</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>१४१७३८</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>परमादेश</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>जिल्ला विकास समितिको कार्यालय कास्की</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>गुदानी कुमार</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>२०७३-१२-१५</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141738.pdf</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>१९</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८५</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>१४१७१९</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>जवरजस्ती करणी</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>डिल्ली स्वार , राकेश कुँवर र ध्रुब कुँवर</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>२०७४-०१-२८</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141719.pdf</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>२०</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१६</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>१४१४८८</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>रतन कुमार श्रेष्ठ</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>मालपोत कार्यालय पर्सा , मालपोत कार्यालय पर्सा , अख्तियार दुरुपयोग अनुसन्धान आयोग टंगाल समेत ६ , लुम्बिनी विकास बैंक लिमिटेड भरतपुर , लुम्बिनी विकास बैंक लिमिटेड मकवानपुर , सुनिता महतो र सुभाषविर माथेमा</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>२०७४-०२-२६</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141488.pdf</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>२१</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१७</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>१४१४९०</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>दिपक कुमार श्रेष्ठ</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>मालपोत कार्यालय पर्सा , अख्तियार दुरुपयोग अनुसन्धान आयोग टंगाल समेत ६ , लुम्बिनी विकास बैंक लिमिटेड भरतपुर , लुम्बिनी विकास बैंक लिमिटेड मकवानपुर , सुनिता महतो र सुभाषविर माथेमा</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>२०७४-०२-२६</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141490.pdf</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>२४</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२७८</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>१४१७२७</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>अशं चलन</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>सुनमाया गुरुङ्गको अ।वा। दिल बहादुर सुनार</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>वीर बहादुर गुरुङ्ग</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>२०७४-०५-०६</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141727.pdf</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>१३</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८८</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>१४१७२५</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>वहुविवाह</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>सन्तोष भन्ने लिला बहादुर गिरी र सम्झना भन्ने रेश्मा गिरी</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>२०७३-०५-२०</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141725.pdf</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>१४</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१८</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>१४१५०५</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>योग बहादुर पाल</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>प्रहरी प्रधान कार्यालय नक्साल समेत ३ र प्रहरी नायव महानिरिक्षक माधव प्रसाद जोशी</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>२०७३-०७-२४</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141505.pdf</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>१५</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८१</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>१४१७३२</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>निषेधाज्ञा</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>मिनादेवी गुप्ता</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>जयकुमार साह</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>२०७३-०६-०६</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141732.pdf</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>१६</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८९</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>१४१७२६</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>कर्तव्य ज्यान</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>लक्ष्मण धमला</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>२०७३-११-०८</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141726.pdf</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>१७</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८४</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>१४१७३६</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>परमादेश</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>जिल्ला प्रहरी कार्यालय मोरंग</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>गुदानी कुमार</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>२०७३-१२-१५</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141736.pdf</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>१८</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२८५</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>१४१७३८</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>परमादेश</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>जिल्ला विकास समितिको कार्यालय कास्की</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>गुदानी कुमार</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>२०७३-१२-१५</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141738.pdf</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>१९</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>०७१-CR-११८५</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>१४१७१९</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>फौजदारी</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>जवरजस्ती करणी</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>डिल्ली स्वार , राकेश कुँवर र ध्रुब कुँवर</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>नेपाल सरकार</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>२०७४-०१-२८</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141719.pdf</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>२०</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१६</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>१४१४८८</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>रतन कुमार श्रेष्ठ</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>मालपोत कार्यालय पर्सा , मालपोत कार्यालय पर्सा , अख्तियार दुरुपयोग अनुसन्धान आयोग टंगाल समेत ६ , लुम्बिनी विकास बैंक लिमिटेड भरतपुर , लुम्बिनी विकास बैंक लिमिटेड मकवानपुर , सुनिता महतो र सुभाषविर माथेमा</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>२०७४-०२-२६</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141488.pdf</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>२१</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>०७१-WO-०८१७</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>१४१४९०</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>रिट निवेदन</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>उत्प्रेषण</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>दिपक कुमार श्रेष्ठ</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>मालपोत कार्यालय पर्सा , अख्तियार दुरुपयोग अनुसन्धान आयोग टंगाल समेत ६ , लुम्बिनी विकास बैंक लिमिटेड भरतपुर , लुम्बिनी विकास बैंक लिमिटेड मकवानपुर , सुनिता महतो र सुभाषविर माथेमा</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>२०७४-०२-२६</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141490.pdf</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>२४</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>०७१-CI-१२७८</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>१४१७२७</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>२०७२-०१-०२</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>देवानी</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>अशं चलन</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>सुनमाया गुरुङ्गको अ।वा। दिल बहादुर सुनार</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>वीर बहादुर गुरुङ्ग</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>२०७४-०५-०६</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>https://supremecourt.gov.np/cp/assets/downloads/supreme_141727.pdf</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>